<commit_message>
final stages of V2 [1]
</commit_message>
<xml_diff>
--- a/SampleLinks.xlsx
+++ b/SampleLinks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Dispersion</t>
-  </si>
-  <si>
-    <t>Snr</t>
   </si>
   <si>
     <t>Tehran</t>
@@ -97,7 +94,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +104,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -168,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -180,6 +183,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -465,7 +471,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,31 +514,29 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1">
         <v>2</v>
@@ -549,19 +553,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1">
         <v>3.6</v>
@@ -578,19 +582,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G4" s="1">
         <v>9.1</v>
@@ -607,19 +611,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="G5" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
final stage of V2 [2]
</commit_message>
<xml_diff>
--- a/SampleLinks.xlsx
+++ b/SampleLinks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -75,10 +75,34 @@
     <t>x+y</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>0.23+0.2</t>
+  </si>
+  <si>
+    <t>x+x</t>
+  </si>
+  <si>
+    <t>2+2</t>
+  </si>
+  <si>
+    <t>3.3+3.3</t>
+  </si>
+  <si>
+    <t>9.1+9.1</t>
+  </si>
+  <si>
+    <t>0.25+0.25</t>
+  </si>
+  <si>
+    <t>0.63+0.63</t>
+  </si>
+  <si>
+    <t>8.1+8.1</t>
+  </si>
+  <si>
+    <t>0.14+0.14</t>
+  </si>
+  <si>
+    <t>1+1</t>
   </si>
 </sst>
 </file>
@@ -471,7 +495,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,16 +560,16 @@
         <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -565,16 +589,16 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.63</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -591,19 +615,19 @@
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1">
-        <v>9.1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>8.1</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -620,19 +644,19 @@
         <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
just for git 2
</commit_message>
<xml_diff>
--- a/SampleLinks.xlsx
+++ b/SampleLinks.xlsx
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -168,6 +168,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -453,7 +456,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,11 +526,12 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
-        <v>0</v>
+      <c r="H2" s="6">
+        <v>1.4E-3</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <f>POWER(4.8434, -27)</f>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -552,11 +556,12 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
-        <v>0</v>
+      <c r="H3" s="6">
+        <v>1.4E-3</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <f t="shared" ref="I3:I6" si="0">POWER(4.8434, -27)</f>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -581,11 +586,12 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1">
-        <v>0</v>
+      <c r="H4" s="6">
+        <v>1.4E-3</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -610,11 +616,12 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="1">
-        <v>0</v>
+      <c r="H5" s="6">
+        <v>1.4E-3</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -639,11 +646,12 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1">
-        <v>0</v>
+      <c r="H6" s="6">
+        <v>1.4E-3</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3.169136089868813E-19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>